<commit_message>
add multiple t test function
</commit_message>
<xml_diff>
--- a/qPCR/format_2.xlsx
+++ b/qPCR/format_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kongmou\Documents\GitHub\my_shiny_apps\qPCR2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kongmou\Desktop\qPCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1468DF2-C921-40BC-90F5-322887868A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A29F3FB-032D-41C0-BC15-F8E25651FE5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2430" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2565" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -526,11 +526,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <f>B5-1</f>
-        <v>21.19</v>
+        <v>19.489999999999998</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:E8" si="0">C5-1</f>
+        <f t="shared" ref="C8:D8" si="0">C5-1</f>
         <v>14.71</v>
       </c>
       <c r="D8" s="1">
@@ -538,8 +537,7 @@
         <v>13.57</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>15.239999999999998</v>
+        <v>12.91</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -547,7 +545,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9:E11" si="1">B6-1</f>
+        <f t="shared" ref="B9:D10" si="1">B6-1</f>
         <v>19.53</v>
       </c>
       <c r="C9" s="1">
@@ -559,8 +557,8 @@
         <v>12.34</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
-        <v>14.11</v>
+        <f>E6-2</f>
+        <v>13.11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -580,8 +578,7 @@
         <v>12.23</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
-        <v>13.75</v>
+        <v>12.96</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>